<commit_message>
Explicitly note that negative values are OK
</commit_message>
<xml_diff>
--- a/templates/data_reportingformat_template.xlsx
+++ b/templates/data_reportingformat_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/penn529/Documents/GitHub/ess-dive-community/essdive-soil-respiration/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFA00AA0-6C1E-3B42-9FB4-68795DCBB77D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{004A1965-7006-374A-A50D-8E78509746EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1480" yWindow="7420" windowWidth="33580" windowHeight="17040" xr2:uid="{A3A4D55E-8452-EA4C-96C7-D53981DE98F4}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16440" xr2:uid="{A3A4D55E-8452-EA4C-96C7-D53981DE98F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -119,9 +119,6 @@
     <t>ISO timestamp END of averaging period (up to a 12-digit integer as specified by the data's temporal resolution)</t>
   </si>
   <si>
-    <t>CO2 flux (positive = to atmosphere)</t>
-  </si>
-  <si>
     <t>Mean chamber CO2 concentration during measurement period</t>
   </si>
   <si>
@@ -240,6 +237,9 @@
   </si>
   <si>
     <t>Stick stuck in chamber.</t>
+  </si>
+  <si>
+    <t>CO2 flux (positive = to atmosphere); negative values are also acceptable</t>
   </si>
 </sst>
 </file>
@@ -713,7 +713,7 @@
   <dimension ref="A1:X37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U11" sqref="U11"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -754,7 +754,7 @@
         <v>14</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I1" s="8" t="s">
         <v>3</v>
@@ -819,126 +819,126 @@
         <v>27</v>
       </c>
       <c r="E2" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="F2" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="G2" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="H2" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="H2" s="11" t="s">
+      <c r="I2" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="I2" s="11" t="s">
+      <c r="J2" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="J2" s="11" t="s">
+      <c r="K2" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="K2" s="11" t="s">
+      <c r="L2" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="L2" s="11" t="s">
+      <c r="M2" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="M2" s="11" t="s">
+      <c r="N2" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="N2" s="11" t="s">
+      <c r="O2" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="O2" s="11" t="s">
+      <c r="P2" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="P2" s="11" t="s">
+      <c r="Q2" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="Q2" s="11" t="s">
+      <c r="R2" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="R2" s="11" t="s">
+      <c r="S2" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="S2" s="11" t="s">
+      <c r="T2" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="T2" s="11" t="s">
+      <c r="U2" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="U2" s="11" t="s">
+      <c r="V2" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="V2" s="11" t="s">
+      <c r="W2" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="W2" s="11" t="s">
+      <c r="X2" s="11" t="s">
         <v>46</v>
-      </c>
-      <c r="X2" s="11" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:24" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F3" s="17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G3" s="17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H3" s="18"/>
       <c r="I3" s="17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J3" s="18"/>
       <c r="K3" s="17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L3" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="M3" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="N3" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="O3" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="M3" s="17" t="s">
+      <c r="P3" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q3" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="R3" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="S3" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="T3" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="U3" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="N3" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="O3" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="P3" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q3" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="R3" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="S3" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="T3" s="17" t="s">
+      <c r="V3" s="20" t="s">
         <v>56</v>
-      </c>
-      <c r="U3" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="V3" s="20" t="s">
-        <v>57</v>
       </c>
       <c r="W3" s="18"/>
       <c r="X3" s="12"/>
@@ -948,7 +948,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C4" s="14">
         <v>20201106115505</v>
@@ -966,13 +966,13 @@
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="H4" s="15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I4" s="15">
         <v>0.88</v>
       </c>
       <c r="J4" s="15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K4" s="15">
         <v>409.8</v>
@@ -999,7 +999,7 @@
         <v>0</v>
       </c>
       <c r="S4" s="15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="T4" s="15">
         <v>0.3</v>
@@ -1014,7 +1014,7 @@
         <v>1</v>
       </c>
       <c r="X4" s="16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.2">
@@ -1022,7 +1022,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C5" s="14">
         <v>2020110611</v>
@@ -1040,7 +1040,7 @@
         <v>2E-3</v>
       </c>
       <c r="H5" s="15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I5" s="15">
         <v>0.9</v>
@@ -1071,7 +1071,7 @@
         <v>2</v>
       </c>
       <c r="S5" s="15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="T5" s="15">
         <v>0.5</v>

</xml_diff>